<commit_message>
delete old file,update api for category and  group management
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1689BB3-7D14-4ED3-99A6-167071136543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4721B4E2-DB66-420D-BC5A-2074BCA36E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9578E655-562C-4104-B8F7-418F8D65ADB7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>state</t>
   </si>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>DISC</t>
+  </si>
+  <si>
+    <t>issue_level</t>
+  </si>
+  <si>
+    <t>External Issue</t>
+  </si>
+  <si>
+    <t>Internal Issue</t>
   </si>
 </sst>
 </file>
@@ -470,13 +479,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C254406F-12FB-4ABC-BFDB-626D932D93E0}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -685,6 +697,28 @@
       </c>
       <c r="C19" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update calendar and branch api
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ifics_be\database\seeders\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AB89E4-3AC8-4D51-9649-99043B3775BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="3585" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>state</t>
   </si>
@@ -41,9 +43,6 @@
     <t>Pahang</t>
   </si>
   <si>
-    <t>Pulau Pinang</t>
-  </si>
-  <si>
     <t>Perak</t>
   </si>
   <si>
@@ -117,13 +116,16 @@
   </si>
   <si>
     <t>Livechat</t>
+  </si>
+  <si>
+    <t>Penang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,7 +143,13 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -154,6 +162,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -162,10 +178,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -445,22 +461,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.85547" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -482,7 +501,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -493,7 +512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -504,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -515,7 +534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -526,7 +545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -534,10 +553,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -545,10 +564,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -556,10 +575,10 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -567,10 +586,10 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -578,10 +597,10 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -589,10 +608,10 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -600,10 +619,10 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -611,10 +630,10 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -622,10 +641,10 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -633,130 +652,131 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>17</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>21</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>24</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
       <c r="C23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>27</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>30</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update operating  time and new command
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE0CAC6-0952-45BA-B66F-FE1B4AE3BE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0B3D43-B1EC-41B4-9270-08F7037F46C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>state</t>
   </si>
@@ -128,6 +128,42 @@
   </si>
   <si>
     <t>Cawangan</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Separuh Hari</t>
+  </si>
+  <si>
+    <t>Hujung Minggu</t>
   </si>
 </sst>
 </file>
@@ -477,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -808,6 +844,116 @@
         <v>35</v>
       </c>
     </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update user,audit and action code
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0B3D43-B1EC-41B4-9270-08F7037F46C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F34CDA-70AC-45CD-A434-E073CD97B66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>state</t>
   </si>
@@ -164,6 +164,18 @@
   </si>
   <si>
     <t>Hujung Minggu</t>
+  </si>
+  <si>
+    <t>action_code_email_recipient</t>
+  </si>
+  <si>
+    <t>To Caller Person| Cc - Active personal in Email UPDT GENERAL GROUP  and  SLA group  | Bcc - Not Available</t>
+  </si>
+  <si>
+    <t>To Selected personal in selected technician group| Cc - Other  active personal in the same selected technician group  | Bcc - Caller Person</t>
+  </si>
+  <si>
+    <t>To Selected personal in selected technician group| Cc - Other  active personal in the same selected technician group  | Bcc - Not Available</t>
   </si>
 </sst>
 </file>
@@ -513,16 +525,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="92.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,6 +966,39 @@
         <v>47</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update sla and sla template update dynamic option
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F34CDA-70AC-45CD-A434-E073CD97B66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B50809-3848-48FB-B34F-E22188F00648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>state</t>
   </si>
@@ -176,6 +176,36 @@
   </si>
   <si>
     <t>To Selected personal in selected technician group| Cc - Other  active personal in the same selected technician group  | Bcc - Not Available</t>
+  </si>
+  <si>
+    <t>sla_type</t>
+  </si>
+  <si>
+    <t>Minit</t>
+  </si>
+  <si>
+    <t>Jam</t>
+  </si>
+  <si>
+    <t>Hari</t>
+  </si>
+  <si>
+    <t>severity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tidak Penting </t>
+  </si>
+  <si>
+    <t>Kritikal</t>
+  </si>
+  <si>
+    <t>Penting</t>
+  </si>
+  <si>
+    <t>Sederhana</t>
+  </si>
+  <si>
+    <t>Rendah</t>
   </si>
 </sst>
 </file>
@@ -525,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1029,96 @@
         <v>51</v>
       </c>
     </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update reftable and user update
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B50809-3848-48FB-B34F-E22188F00648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6250F720-DA3A-4CD1-9696-89E4E4167244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,15 +169,6 @@
     <t>action_code_email_recipient</t>
   </si>
   <si>
-    <t>To Caller Person| Cc - Active personal in Email UPDT GENERAL GROUP  and  SLA group  | Bcc - Not Available</t>
-  </si>
-  <si>
-    <t>To Selected personal in selected technician group| Cc - Other  active personal in the same selected technician group  | Bcc - Caller Person</t>
-  </si>
-  <si>
-    <t>To Selected personal in selected technician group| Cc - Other  active personal in the same selected technician group  | Bcc - Not Available</t>
-  </si>
-  <si>
     <t>sla_type</t>
   </si>
   <si>
@@ -206,6 +197,15 @@
   </si>
   <si>
     <t>Rendah</t>
+  </si>
+  <si>
+    <t>To: Pengadu, CC: Kumpulan yang berkaitan BCC: Tidak Berkenaan</t>
+  </si>
+  <si>
+    <t>To: Juruteknik yang berkaitan, CC: Kumpulan Juruteknik yang berkaitan BC: Pengadu</t>
+  </si>
+  <si>
+    <t>To: Juruteknik yang berkaitan, CC: Kumpulan Juruteknik yang berkaitan BCC: Tidak Berkenaan</t>
   </si>
 </sst>
 </file>
@@ -558,7 +558,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1004,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1026,95 +1026,95 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B45">
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B48">
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B49">
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B50">
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create new api incident and incident solution
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6250F720-DA3A-4CD1-9696-89E4E4167244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F8081-93D0-4CFD-9CFE-BAE942A09739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t>state</t>
   </si>
@@ -206,6 +206,30 @@
   </si>
   <si>
     <t>To: Juruteknik yang berkaitan, CC: Kumpulan Juruteknik yang berkaitan BCC: Tidak Berkenaan</t>
+  </si>
+  <si>
+    <t>incident_asset_type</t>
+  </si>
+  <si>
+    <t>Hilang</t>
+  </si>
+  <si>
+    <t>Rosak</t>
+  </si>
+  <si>
+    <t>received_via</t>
+  </si>
+  <si>
+    <t>Telefon</t>
+  </si>
+  <si>
+    <t>Emel</t>
+  </si>
+  <si>
+    <t>Chatbot</t>
+  </si>
+  <si>
+    <t>Live Chat</t>
   </si>
 </sst>
 </file>
@@ -555,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,6 +1141,72 @@
         <v>58</v>
       </c>
     </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>62</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>4</v>
+      </c>
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update reftable and sla
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67F8081-93D0-4CFD-9CFE-BAE942A09739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83092F3C-FF6E-41BA-A2FE-3FF84AA1E0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
   <si>
     <t>state</t>
   </si>
@@ -230,6 +230,117 @@
   </si>
   <si>
     <t>Live Chat</t>
+  </si>
+  <si>
+    <t>RM 500</t>
+  </si>
+  <si>
+    <t>RM 200</t>
+  </si>
+  <si>
+    <t>RM 10000</t>
+  </si>
+  <si>
+    <t>RM 5000</t>
+  </si>
+  <si>
+    <t>RM 3000</t>
+  </si>
+  <si>
+    <t>RM 1000</t>
+  </si>
+  <si>
+    <t>penalty_price</t>
+  </si>
+  <si>
+    <t>Isu Dalaman</t>
+  </si>
+  <si>
+    <t>Isu Luaran</t>
+  </si>
+  <si>
+    <t>Aktif</t>
+  </si>
+  <si>
+    <t>Tidak Aktif</t>
+  </si>
+  <si>
+    <t>Tidak Kritikal</t>
+  </si>
+  <si>
+    <t>E-mel</t>
+  </si>
+  <si>
+    <t>Sembang Langsung</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>Isnin</t>
+  </si>
+  <si>
+    <t>Selasa</t>
+  </si>
+  <si>
+    <t>Rabu</t>
+  </si>
+  <si>
+    <t>Khamis</t>
+  </si>
+  <si>
+    <t>Jumaat</t>
+  </si>
+  <si>
+    <t>Sabtu</t>
+  </si>
+  <si>
+    <t>Ahad</t>
+  </si>
+  <si>
+    <t>Half Day</t>
+  </si>
+  <si>
+    <t>Weekend</t>
+  </si>
+  <si>
+    <t>To: Complainant, CC: Relevant Group, BCC: Not Applicable</t>
+  </si>
+  <si>
+    <t>To: Relevant Technician, CC: Relevant Technician Group, BCC: Complainant</t>
+  </si>
+  <si>
+    <t>To: Relevant Technician, CC: Relevant Technician Group, BCC: Not Applicable</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Not Important</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>Moderate</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Damaged / Broken</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -265,8 +376,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,19 +693,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="3" max="3" width="92.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,8 +716,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -612,8 +730,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -623,8 +744,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -634,8 +758,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -645,8 +772,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -656,8 +786,11 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -667,8 +800,11 @@
       <c r="C7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -678,8 +814,11 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -689,8 +828,11 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -700,8 +842,11 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -711,8 +856,11 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -722,8 +870,11 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -733,8 +884,11 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -744,8 +898,11 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -755,8 +912,11 @@
       <c r="C15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -766,8 +926,11 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -777,8 +940,11 @@
       <c r="C17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -788,8 +954,11 @@
       <c r="C18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -799,8 +968,11 @@
       <c r="C19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -810,8 +982,11 @@
       <c r="C20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -821,8 +996,11 @@
       <c r="C21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -832,8 +1010,11 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -843,8 +1024,11 @@
       <c r="C23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -854,8 +1038,11 @@
       <c r="C24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -865,8 +1052,11 @@
       <c r="C25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -876,8 +1066,11 @@
       <c r="C26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -887,8 +1080,11 @@
       <c r="C27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -898,8 +1094,11 @@
       <c r="C28" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -907,10 +1106,13 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -920,8 +1122,11 @@
       <c r="C30" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -931,8 +1136,11 @@
       <c r="C31" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -942,8 +1150,11 @@
       <c r="C32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -953,8 +1164,11 @@
       <c r="C33" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -964,8 +1178,11 @@
       <c r="C34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -975,8 +1192,11 @@
       <c r="C35" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -986,8 +1206,11 @@
       <c r="C36" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -997,8 +1220,11 @@
       <c r="C37" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1006,10 +1232,13 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>44</v>
       </c>
@@ -1017,10 +1246,13 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1028,10 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1039,10 +1274,13 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1050,10 +1288,13 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1061,10 +1302,13 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1072,10 +1316,13 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1083,10 +1330,13 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -1094,10 +1344,13 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -1105,10 +1358,13 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -1116,10 +1372,13 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -1127,10 +1386,13 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
+        <v>102</v>
+      </c>
+      <c r="D49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1138,10 +1400,13 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -1149,10 +1414,13 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
+        <v>104</v>
+      </c>
+      <c r="D51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>62</v>
       </c>
@@ -1160,10 +1428,13 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
+        <v>105</v>
+      </c>
+      <c r="D52" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -1171,10 +1442,13 @@
         <v>1</v>
       </c>
       <c r="C53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -1182,10 +1456,13 @@
         <v>2</v>
       </c>
       <c r="C54" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -1195,16 +1472,142 @@
       <c r="C55" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>69</v>
+      </c>
+      <c r="D56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" t="s">
+        <v>53</v>
+      </c>
+      <c r="F57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58" t="s">
+        <v>73</v>
+      </c>
+      <c r="D58" t="s">
+        <v>73</v>
+      </c>
+      <c r="E58" t="s">
+        <v>53</v>
+      </c>
+      <c r="F58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>74</v>
+      </c>
+      <c r="D59" t="s">
+        <v>74</v>
+      </c>
+      <c r="E59" t="s">
+        <v>53</v>
+      </c>
+      <c r="F59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60">
+        <v>4</v>
+      </c>
+      <c r="C60" t="s">
+        <v>75</v>
+      </c>
+      <c r="D60" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" t="s">
+        <v>53</v>
+      </c>
+      <c r="F60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>76</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+      <c r="C61" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" t="s">
+        <v>70</v>
+      </c>
+      <c r="E61" t="s">
+        <v>53</v>
+      </c>
+      <c r="F61" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>71</v>
+      </c>
+      <c r="D62" t="s">
+        <v>71</v>
+      </c>
+      <c r="E62" t="s">
+        <v>53</v>
+      </c>
+      <c r="F62" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update reftable and incident
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83092F3C-FF6E-41BA-A2FE-3FF84AA1E0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEE5C62-3EFC-40A0-B0B5-0198D02304DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4620" yWindow="2595" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="117">
   <si>
     <t>state</t>
   </si>
@@ -184,21 +184,9 @@
     <t>severity</t>
   </si>
   <si>
-    <t xml:space="preserve">Tidak Penting </t>
-  </si>
-  <si>
     <t>Kritikal</t>
   </si>
   <si>
-    <t>Penting</t>
-  </si>
-  <si>
-    <t>Sederhana</t>
-  </si>
-  <si>
-    <t>Rendah</t>
-  </si>
-  <si>
     <t>To: Pengadu, CC: Kumpulan yang berkaitan BCC: Tidak Berkenaan</t>
   </si>
   <si>
@@ -328,12 +316,6 @@
     <t>Important</t>
   </si>
   <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>Missing</t>
   </si>
   <si>
@@ -341,6 +323,54 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>0- Tidak Penting</t>
+  </si>
+  <si>
+    <t>0- Not Important</t>
+  </si>
+  <si>
+    <t>1- Kritikal</t>
+  </si>
+  <si>
+    <t>1- Critical</t>
+  </si>
+  <si>
+    <t>2- Important</t>
+  </si>
+  <si>
+    <t>2- Penting</t>
+  </si>
+  <si>
+    <t>3- Sederhana</t>
+  </si>
+  <si>
+    <t>3- Medium</t>
+  </si>
+  <si>
+    <t>4- Low</t>
+  </si>
+  <si>
+    <t>4- Rendah</t>
+  </si>
+  <si>
+    <t>loaner_type</t>
+  </si>
+  <si>
+    <t>Minggu</t>
+  </si>
+  <si>
+    <t>Bulan</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Week</t>
+  </si>
+  <si>
+    <t>Month</t>
   </si>
 </sst>
 </file>
@@ -693,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +1013,7 @@
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -997,7 +1027,7 @@
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1011,7 +1041,7 @@
         <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1025,7 +1055,7 @@
         <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1039,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,7 +1083,7 @@
         <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1067,7 +1097,7 @@
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,7 +1111,7 @@
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1106,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
@@ -1123,7 +1153,7 @@
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1167,7 @@
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,7 +1181,7 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,7 +1195,7 @@
         <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,7 +1209,7 @@
         <v>41</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1193,7 +1223,7 @@
         <v>42</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1207,7 +1237,7 @@
         <v>43</v>
       </c>
       <c r="D36" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,7 +1262,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D38" t="s">
         <v>46</v>
@@ -1246,7 +1276,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
         <v>47</v>
@@ -1260,10 +1290,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1274,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D41" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,10 +1318,10 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1302,7 +1332,7 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D43" t="s">
         <v>50</v>
@@ -1316,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D44" t="s">
         <v>51</v>
@@ -1330,7 +1360,7 @@
         <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
         <v>52</v>
@@ -1344,10 +1374,10 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,10 +1388,10 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>27</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1372,10 +1402,10 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,10 +1416,10 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,57 +1430,57 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -1459,69 +1489,69 @@
         <v>30</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E57" t="s">
         <v>53</v>
       </c>
       <c r="F57" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B58">
         <v>2</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E58" t="s">
         <v>53</v>
@@ -1532,56 +1562,56 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E59" t="s">
         <v>53</v>
       </c>
       <c r="F59" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B60">
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E60" t="s">
         <v>53</v>
       </c>
       <c r="F60" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B61">
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D61" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E61" t="s">
         <v>53</v>
@@ -1592,22 +1622,64 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B62">
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D62" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
         <v>53</v>
       </c>
       <c r="F62" t="s">
-        <v>101</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>114</v>
+      </c>
+      <c r="D63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>116</v>
+      </c>
+      <c r="D65" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update incident complaint and email
</commit_message>
<xml_diff>
--- a/database/seeders/excel/ref_table.xlsx
+++ b/database/seeders/excel/ref_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ifics_be\database\seeders\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8BBA96-C6AC-4A33-A10B-51A688894D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0CA72F-7AEF-4A9A-84EE-0AC32D00546A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -740,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,10 +1459,10 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1473,10 +1473,10 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>